<commit_message>
Additions to readme including analysis
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\anony\Dropbox\Case Western\2019-2020\Fall\Networks\Projects\Project 2\rawsocket-distance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7A07A0-A133-42AA-A57A-913B06EC508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3CECB3-C480-4F13-B5BF-732B4D58AC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>site</t>
-  </si>
-  <si>
-    <t>hops</t>
   </si>
   <si>
     <t>time</t>
@@ -71,6 +76,30 @@
   </si>
   <si>
     <t>rambler.ru</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
+  <si>
+    <t>Std Deviation:</t>
+  </si>
+  <si>
+    <t>Low Average</t>
+  </si>
+  <si>
+    <t>Low Std. Dev</t>
+  </si>
+  <si>
+    <t>High Std. Dev</t>
+  </si>
+  <si>
+    <t>High Average</t>
+  </si>
+  <si>
+    <t>hops to target</t>
+  </si>
+  <si>
+    <t>time/hop (corrected)</t>
   </si>
 </sst>
 </file>
@@ -2402,16 +2431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2736,43 +2765,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -2789,10 +2824,14 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
+      <c r="G2">
+        <f>C2/(B2*2)</f>
+        <v>2.5208333333333333E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>16</v>
@@ -2809,10 +2848,14 @@
       <c r="F3" t="b">
         <v>1</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="0">C3/(B3*2)</f>
+        <v>2.6994687499999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -2829,10 +2872,14 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>3.3055555555555553E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -2849,10 +2896,14 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4.8094615384615391</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -2869,10 +2920,14 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.7269318181818183</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -2889,10 +2944,14 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.1833333333333332E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -2909,10 +2968,14 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.8400000000000004E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -2929,10 +2992,14 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3.2592105263157891</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -2949,10 +3016,14 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>5.3849999999999995E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -2969,10 +3040,14 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3.6777777777777777E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>19</v>
@@ -2988,6 +3063,64 @@
       </c>
       <c r="F12" t="b">
         <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.1856315789473686</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <f>AVERAGE(G2:G12)</f>
+        <v>1.5363481101733194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <f>_xlfn.STDEV.P(G2:G12)</f>
+        <v>1.7233518761999724</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <f>AVERAGE(G2,G4,G7,G8,G10,G11)</f>
+        <v>3.6520833333333329E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.STDEV.S(G2,G4,G7,G10,G11)</f>
+        <v>1.0742593342782488E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20">
+        <f>AVERAGE(G3,G5,G6,G9,G12)</f>
+        <v>3.3361408423813024</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <f>_xlfn.STDEV.S(G5,G3,G6,G9,G12)</f>
+        <v>0.86251553229362321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>